<commit_message>
Toán tử ++ --
</commit_message>
<xml_diff>
--- a/1.nen-tang-lap-trinh-java/2.Bien-so-hang-so-va-kieu-du-lieu.xlsx
+++ b/1.nen-tang-lap-trinh-java/2.Bien-so-hang-so-va-kieu-du-lieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\java\1.nen-tang-lap-trinh-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD1F06B-772B-4354-A440-06882D16BB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FBD0D2-D1D6-40A2-8EC7-6AFB5BC11890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="1050" windowWidth="25215" windowHeight="13350" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31440" yWindow="1560" windowWidth="25215" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Package &amp; Eclipe preferences" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="156">
   <si>
     <r>
       <t>T</t>
@@ -5546,6 +5546,10 @@
       </rPr>
       <t>ng)</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Endcoding</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5767,7 +5771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -5784,8 +5788,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -6509,6 +6511,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>407</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>535531</xdr:colOff>
+      <xdr:row>433</xdr:row>
+      <xdr:rowOff>37359</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="図 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0614882A-11D8-0797-18FB-3A27E70B4B8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="93097350"/>
+          <a:ext cx="8355556" cy="5923809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7147,10 +7193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:T404"/>
+  <dimension ref="B3:T434"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
+      <selection activeCell="Q406" sqref="Q406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -8686,19 +8732,19 @@
       <c r="B400" s="4"/>
       <c r="J400" s="5"/>
     </row>
-    <row r="401" spans="2:10">
+    <row r="401" spans="2:14">
       <c r="B401" s="4"/>
       <c r="J401" s="5"/>
     </row>
-    <row r="402" spans="2:10">
+    <row r="402" spans="2:14">
       <c r="B402" s="4"/>
       <c r="J402" s="5"/>
     </row>
-    <row r="403" spans="2:10">
+    <row r="403" spans="2:14">
       <c r="B403" s="4"/>
       <c r="J403" s="5"/>
     </row>
-    <row r="404" spans="2:10">
+    <row r="404" spans="2:14">
       <c r="B404" s="6"/>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
@@ -8708,6 +8754,428 @@
       <c r="H404" s="7"/>
       <c r="I404" s="7"/>
       <c r="J404" s="8"/>
+    </row>
+    <row r="407" spans="2:14">
+      <c r="B407" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C407" s="2"/>
+      <c r="D407" s="2"/>
+      <c r="E407" s="2"/>
+      <c r="F407" s="2"/>
+      <c r="G407" s="2"/>
+      <c r="H407" s="2"/>
+      <c r="I407" s="2"/>
+      <c r="J407" s="2"/>
+      <c r="K407" s="2"/>
+      <c r="L407" s="2"/>
+      <c r="M407" s="2"/>
+      <c r="N407" s="3"/>
+    </row>
+    <row r="408" spans="2:14">
+      <c r="B408" s="4"/>
+      <c r="C408" s="15"/>
+      <c r="D408" s="15"/>
+      <c r="E408" s="15"/>
+      <c r="F408" s="15"/>
+      <c r="G408" s="15"/>
+      <c r="H408" s="15"/>
+      <c r="I408" s="15"/>
+      <c r="J408" s="15"/>
+      <c r="K408" s="15"/>
+      <c r="L408" s="15"/>
+      <c r="M408" s="15"/>
+      <c r="N408" s="5"/>
+    </row>
+    <row r="409" spans="2:14">
+      <c r="B409" s="4"/>
+      <c r="C409" s="15"/>
+      <c r="D409" s="15"/>
+      <c r="E409" s="15"/>
+      <c r="F409" s="15"/>
+      <c r="G409" s="15"/>
+      <c r="H409" s="15"/>
+      <c r="I409" s="15"/>
+      <c r="J409" s="15"/>
+      <c r="K409" s="15"/>
+      <c r="L409" s="15"/>
+      <c r="M409" s="15"/>
+      <c r="N409" s="5"/>
+    </row>
+    <row r="410" spans="2:14">
+      <c r="B410" s="4"/>
+      <c r="C410" s="15"/>
+      <c r="D410" s="15"/>
+      <c r="E410" s="15"/>
+      <c r="F410" s="15"/>
+      <c r="G410" s="15"/>
+      <c r="H410" s="15"/>
+      <c r="I410" s="15"/>
+      <c r="J410" s="15"/>
+      <c r="K410" s="15"/>
+      <c r="L410" s="15"/>
+      <c r="M410" s="15"/>
+      <c r="N410" s="5"/>
+    </row>
+    <row r="411" spans="2:14">
+      <c r="B411" s="4"/>
+      <c r="C411" s="15"/>
+      <c r="D411" s="15"/>
+      <c r="E411" s="15"/>
+      <c r="F411" s="15"/>
+      <c r="G411" s="15"/>
+      <c r="H411" s="15"/>
+      <c r="I411" s="15"/>
+      <c r="J411" s="15"/>
+      <c r="K411" s="15"/>
+      <c r="L411" s="15"/>
+      <c r="M411" s="15"/>
+      <c r="N411" s="5"/>
+    </row>
+    <row r="412" spans="2:14">
+      <c r="B412" s="4"/>
+      <c r="C412" s="15"/>
+      <c r="D412" s="15"/>
+      <c r="E412" s="15"/>
+      <c r="F412" s="15"/>
+      <c r="G412" s="15"/>
+      <c r="H412" s="15"/>
+      <c r="I412" s="15"/>
+      <c r="J412" s="15"/>
+      <c r="K412" s="15"/>
+      <c r="L412" s="15"/>
+      <c r="M412" s="15"/>
+      <c r="N412" s="5"/>
+    </row>
+    <row r="413" spans="2:14">
+      <c r="B413" s="4"/>
+      <c r="C413" s="15"/>
+      <c r="D413" s="15"/>
+      <c r="E413" s="15"/>
+      <c r="F413" s="15"/>
+      <c r="G413" s="15"/>
+      <c r="H413" s="15"/>
+      <c r="I413" s="15"/>
+      <c r="J413" s="15"/>
+      <c r="K413" s="15"/>
+      <c r="L413" s="15"/>
+      <c r="M413" s="15"/>
+      <c r="N413" s="5"/>
+    </row>
+    <row r="414" spans="2:14">
+      <c r="B414" s="4"/>
+      <c r="C414" s="15"/>
+      <c r="D414" s="15"/>
+      <c r="E414" s="15"/>
+      <c r="F414" s="15"/>
+      <c r="G414" s="15"/>
+      <c r="H414" s="15"/>
+      <c r="I414" s="15"/>
+      <c r="J414" s="15"/>
+      <c r="K414" s="15"/>
+      <c r="L414" s="15"/>
+      <c r="M414" s="15"/>
+      <c r="N414" s="5"/>
+    </row>
+    <row r="415" spans="2:14">
+      <c r="B415" s="4"/>
+      <c r="C415" s="15"/>
+      <c r="D415" s="15"/>
+      <c r="E415" s="15"/>
+      <c r="F415" s="15"/>
+      <c r="G415" s="15"/>
+      <c r="H415" s="15"/>
+      <c r="I415" s="15"/>
+      <c r="J415" s="15"/>
+      <c r="K415" s="15"/>
+      <c r="L415" s="15"/>
+      <c r="M415" s="15"/>
+      <c r="N415" s="5"/>
+    </row>
+    <row r="416" spans="2:14">
+      <c r="B416" s="4"/>
+      <c r="C416" s="15"/>
+      <c r="D416" s="15"/>
+      <c r="E416" s="15"/>
+      <c r="F416" s="15"/>
+      <c r="G416" s="15"/>
+      <c r="H416" s="15"/>
+      <c r="I416" s="15"/>
+      <c r="J416" s="15"/>
+      <c r="K416" s="15"/>
+      <c r="L416" s="15"/>
+      <c r="M416" s="15"/>
+      <c r="N416" s="5"/>
+    </row>
+    <row r="417" spans="2:14">
+      <c r="B417" s="4"/>
+      <c r="C417" s="15"/>
+      <c r="D417" s="15"/>
+      <c r="E417" s="15"/>
+      <c r="F417" s="15"/>
+      <c r="G417" s="15"/>
+      <c r="H417" s="15"/>
+      <c r="I417" s="15"/>
+      <c r="J417" s="15"/>
+      <c r="K417" s="15"/>
+      <c r="L417" s="15"/>
+      <c r="M417" s="15"/>
+      <c r="N417" s="5"/>
+    </row>
+    <row r="418" spans="2:14">
+      <c r="B418" s="4"/>
+      <c r="C418" s="15"/>
+      <c r="D418" s="15"/>
+      <c r="E418" s="15"/>
+      <c r="F418" s="15"/>
+      <c r="G418" s="15"/>
+      <c r="H418" s="15"/>
+      <c r="I418" s="15"/>
+      <c r="J418" s="15"/>
+      <c r="K418" s="15"/>
+      <c r="L418" s="15"/>
+      <c r="M418" s="15"/>
+      <c r="N418" s="5"/>
+    </row>
+    <row r="419" spans="2:14">
+      <c r="B419" s="4"/>
+      <c r="C419" s="15"/>
+      <c r="D419" s="15"/>
+      <c r="E419" s="15"/>
+      <c r="F419" s="15"/>
+      <c r="G419" s="15"/>
+      <c r="H419" s="15"/>
+      <c r="I419" s="15"/>
+      <c r="J419" s="15"/>
+      <c r="K419" s="15"/>
+      <c r="L419" s="15"/>
+      <c r="M419" s="15"/>
+      <c r="N419" s="5"/>
+    </row>
+    <row r="420" spans="2:14">
+      <c r="B420" s="4"/>
+      <c r="C420" s="15"/>
+      <c r="D420" s="15"/>
+      <c r="E420" s="15"/>
+      <c r="F420" s="15"/>
+      <c r="G420" s="15"/>
+      <c r="H420" s="15"/>
+      <c r="I420" s="15"/>
+      <c r="J420" s="15"/>
+      <c r="K420" s="15"/>
+      <c r="L420" s="15"/>
+      <c r="M420" s="15"/>
+      <c r="N420" s="5"/>
+    </row>
+    <row r="421" spans="2:14">
+      <c r="B421" s="4"/>
+      <c r="C421" s="15"/>
+      <c r="D421" s="15"/>
+      <c r="E421" s="15"/>
+      <c r="F421" s="15"/>
+      <c r="G421" s="15"/>
+      <c r="H421" s="15"/>
+      <c r="I421" s="15"/>
+      <c r="J421" s="15"/>
+      <c r="K421" s="15"/>
+      <c r="L421" s="15"/>
+      <c r="M421" s="15"/>
+      <c r="N421" s="5"/>
+    </row>
+    <row r="422" spans="2:14">
+      <c r="B422" s="4"/>
+      <c r="C422" s="15"/>
+      <c r="D422" s="15"/>
+      <c r="E422" s="15"/>
+      <c r="F422" s="15"/>
+      <c r="G422" s="15"/>
+      <c r="H422" s="15"/>
+      <c r="I422" s="15"/>
+      <c r="J422" s="15"/>
+      <c r="K422" s="15"/>
+      <c r="L422" s="15"/>
+      <c r="M422" s="15"/>
+      <c r="N422" s="5"/>
+    </row>
+    <row r="423" spans="2:14">
+      <c r="B423" s="4"/>
+      <c r="C423" s="15"/>
+      <c r="D423" s="15"/>
+      <c r="E423" s="15"/>
+      <c r="F423" s="15"/>
+      <c r="G423" s="15"/>
+      <c r="H423" s="15"/>
+      <c r="I423" s="15"/>
+      <c r="J423" s="15"/>
+      <c r="K423" s="15"/>
+      <c r="L423" s="15"/>
+      <c r="M423" s="15"/>
+      <c r="N423" s="5"/>
+    </row>
+    <row r="424" spans="2:14">
+      <c r="B424" s="4"/>
+      <c r="C424" s="15"/>
+      <c r="D424" s="15"/>
+      <c r="E424" s="15"/>
+      <c r="F424" s="15"/>
+      <c r="G424" s="15"/>
+      <c r="H424" s="15"/>
+      <c r="I424" s="15"/>
+      <c r="J424" s="15"/>
+      <c r="K424" s="15"/>
+      <c r="L424" s="15"/>
+      <c r="M424" s="15"/>
+      <c r="N424" s="5"/>
+    </row>
+    <row r="425" spans="2:14">
+      <c r="B425" s="4"/>
+      <c r="C425" s="15"/>
+      <c r="D425" s="15"/>
+      <c r="E425" s="15"/>
+      <c r="F425" s="15"/>
+      <c r="G425" s="15"/>
+      <c r="H425" s="15"/>
+      <c r="I425" s="15"/>
+      <c r="J425" s="15"/>
+      <c r="K425" s="15"/>
+      <c r="L425" s="15"/>
+      <c r="M425" s="15"/>
+      <c r="N425" s="5"/>
+    </row>
+    <row r="426" spans="2:14">
+      <c r="B426" s="4"/>
+      <c r="C426" s="15"/>
+      <c r="D426" s="15"/>
+      <c r="E426" s="15"/>
+      <c r="F426" s="15"/>
+      <c r="G426" s="15"/>
+      <c r="H426" s="15"/>
+      <c r="I426" s="15"/>
+      <c r="J426" s="15"/>
+      <c r="K426" s="15"/>
+      <c r="L426" s="15"/>
+      <c r="M426" s="15"/>
+      <c r="N426" s="5"/>
+    </row>
+    <row r="427" spans="2:14">
+      <c r="B427" s="4"/>
+      <c r="C427" s="15"/>
+      <c r="D427" s="15"/>
+      <c r="E427" s="15"/>
+      <c r="F427" s="15"/>
+      <c r="G427" s="15"/>
+      <c r="H427" s="15"/>
+      <c r="I427" s="15"/>
+      <c r="J427" s="15"/>
+      <c r="K427" s="15"/>
+      <c r="L427" s="15"/>
+      <c r="M427" s="15"/>
+      <c r="N427" s="5"/>
+    </row>
+    <row r="428" spans="2:14">
+      <c r="B428" s="4"/>
+      <c r="C428" s="15"/>
+      <c r="D428" s="15"/>
+      <c r="E428" s="15"/>
+      <c r="F428" s="15"/>
+      <c r="G428" s="15"/>
+      <c r="H428" s="15"/>
+      <c r="I428" s="15"/>
+      <c r="J428" s="15"/>
+      <c r="K428" s="15"/>
+      <c r="L428" s="15"/>
+      <c r="M428" s="15"/>
+      <c r="N428" s="5"/>
+    </row>
+    <row r="429" spans="2:14">
+      <c r="B429" s="4"/>
+      <c r="C429" s="15"/>
+      <c r="D429" s="15"/>
+      <c r="E429" s="15"/>
+      <c r="F429" s="15"/>
+      <c r="G429" s="15"/>
+      <c r="H429" s="15"/>
+      <c r="I429" s="15"/>
+      <c r="J429" s="15"/>
+      <c r="K429" s="15"/>
+      <c r="L429" s="15"/>
+      <c r="M429" s="15"/>
+      <c r="N429" s="5"/>
+    </row>
+    <row r="430" spans="2:14">
+      <c r="B430" s="4"/>
+      <c r="C430" s="15"/>
+      <c r="D430" s="15"/>
+      <c r="E430" s="15"/>
+      <c r="F430" s="15"/>
+      <c r="G430" s="15"/>
+      <c r="H430" s="15"/>
+      <c r="I430" s="15"/>
+      <c r="J430" s="15"/>
+      <c r="K430" s="15"/>
+      <c r="L430" s="15"/>
+      <c r="M430" s="15"/>
+      <c r="N430" s="5"/>
+    </row>
+    <row r="431" spans="2:14">
+      <c r="B431" s="4"/>
+      <c r="C431" s="15"/>
+      <c r="D431" s="15"/>
+      <c r="E431" s="15"/>
+      <c r="F431" s="15"/>
+      <c r="G431" s="15"/>
+      <c r="H431" s="15"/>
+      <c r="I431" s="15"/>
+      <c r="J431" s="15"/>
+      <c r="K431" s="15"/>
+      <c r="L431" s="15"/>
+      <c r="M431" s="15"/>
+      <c r="N431" s="5"/>
+    </row>
+    <row r="432" spans="2:14">
+      <c r="B432" s="4"/>
+      <c r="C432" s="15"/>
+      <c r="D432" s="15"/>
+      <c r="E432" s="15"/>
+      <c r="F432" s="15"/>
+      <c r="G432" s="15"/>
+      <c r="H432" s="15"/>
+      <c r="I432" s="15"/>
+      <c r="J432" s="15"/>
+      <c r="K432" s="15"/>
+      <c r="L432" s="15"/>
+      <c r="M432" s="15"/>
+      <c r="N432" s="5"/>
+    </row>
+    <row r="433" spans="2:14">
+      <c r="B433" s="4"/>
+      <c r="C433" s="15"/>
+      <c r="D433" s="15"/>
+      <c r="E433" s="15"/>
+      <c r="F433" s="15"/>
+      <c r="G433" s="15"/>
+      <c r="H433" s="15"/>
+      <c r="I433" s="15"/>
+      <c r="J433" s="15"/>
+      <c r="K433" s="15"/>
+      <c r="L433" s="15"/>
+      <c r="M433" s="15"/>
+      <c r="N433" s="5"/>
+    </row>
+    <row r="434" spans="2:14">
+      <c r="B434" s="6"/>
+      <c r="C434" s="7"/>
+      <c r="D434" s="7"/>
+      <c r="E434" s="7"/>
+      <c r="F434" s="7"/>
+      <c r="G434" s="7"/>
+      <c r="H434" s="7"/>
+      <c r="I434" s="7"/>
+      <c r="J434" s="7"/>
+      <c r="K434" s="7"/>
+      <c r="L434" s="7"/>
+      <c r="M434" s="7"/>
+      <c r="N434" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -10504,7 +10972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9F4B46-6B44-4169-878D-942F3071F7E6}">
   <dimension ref="B3:M160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -10624,77 +11092,47 @@
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="4"/>
-      <c r="C26" s="15" t="s">
+      <c r="C26" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="4"/>
-      <c r="C27" s="15" t="s">
+      <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="4"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="4"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="4"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
       <c r="H30" s="5"/>
       <c r="I30" t="s">
         <v>35</v>
@@ -10705,13 +11143,9 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="4"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
       <c r="H31" s="5"/>
       <c r="I31" t="s">
         <v>35</v>
@@ -10722,625 +11156,405 @@
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="4"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="D32" s="12"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="4"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="4"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="4"/>
-      <c r="C35" s="15" t="s">
+      <c r="C35" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="4"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="4"/>
-      <c r="C37" s="15" t="s">
+      <c r="C37" t="s">
         <v>139</v>
       </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="4"/>
-      <c r="C38" s="15" t="s">
+      <c r="C38" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="4"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15" t="s">
+      <c r="D39" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" t="s">
         <v>142</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="4"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15" t="s">
+      <c r="D40" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" t="s">
         <v>144</v>
       </c>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="4"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15" t="s">
+      <c r="D41" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="4"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15" t="s">
+      <c r="D42" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="4"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="D43" t="s">
         <v>147</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="4"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="4"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15" t="s">
+      <c r="D45" t="s">
         <v>148</v>
       </c>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="4"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15" t="s">
+      <c r="D46" t="s">
         <v>149</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="4"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15" t="s">
+      <c r="D47" t="s">
         <v>137</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="4"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15" t="s">
+      <c r="D48" t="s">
         <v>138</v>
       </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="4"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15" t="s">
+      <c r="D49" t="s">
         <v>48</v>
       </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="4"/>
-      <c r="C50" s="15" t="s">
+      <c r="C50" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="4"/>
-      <c r="C51" s="15" t="s">
+      <c r="C51" t="s">
         <v>150</v>
       </c>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="4"/>
-      <c r="C52" s="15" t="s">
+      <c r="C52" t="s">
         <v>151</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="2:8">
       <c r="B53" s="4"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15" t="s">
+      <c r="D53" t="s">
         <v>56</v>
       </c>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="2:8">
       <c r="B54" s="4"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15" t="s">
+      <c r="D54" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="4"/>
-      <c r="C55" s="15" t="s">
+      <c r="C55" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="4"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="4"/>
-      <c r="C57" s="15" t="s">
+      <c r="C57" t="s">
         <v>58</v>
       </c>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="2:8">
       <c r="B58" s="4"/>
-      <c r="C58" s="15" t="s">
+      <c r="C58" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="2:8">
       <c r="B59" s="4"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15" t="s">
+      <c r="D59" t="s">
         <v>14</v>
       </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="2:8">
       <c r="B60" s="4"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15" t="s">
+      <c r="D60" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="2:8">
       <c r="B61" s="4"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15" t="s">
+      <c r="D61" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="2:8">
       <c r="B62" s="4"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15" t="s">
+      <c r="D62" t="s">
         <v>21</v>
       </c>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="4"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15" t="s">
+      <c r="D63" t="s">
         <v>22</v>
       </c>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="2:8">
       <c r="B64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15" t="s">
+      <c r="D64" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15" t="s">
+      <c r="D65" t="s">
         <v>25</v>
       </c>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15" t="s">
+      <c r="D66" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="2:8">
       <c r="B67" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15" t="s">
+      <c r="D67" t="s">
         <v>27</v>
       </c>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="2:8">
       <c r="B68" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15" t="s">
+      <c r="D68" t="s">
         <v>28</v>
       </c>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="2:8">
       <c r="B69" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15" t="s">
+      <c r="D69" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="2:8">
       <c r="B70" s="4"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="2:8">
       <c r="B71" s="4"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15" t="s">
+      <c r="D71" t="s">
         <v>30</v>
       </c>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
       <c r="H71" s="5"/>
     </row>
     <row r="72" spans="2:8">
       <c r="B72" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15" t="s">
+      <c r="D72" t="s">
         <v>31</v>
       </c>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15" t="s">
+      <c r="F72" t="s">
         <v>32</v>
       </c>
-      <c r="G72" s="15"/>
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="2:8">
       <c r="B73" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15" t="s">
+      <c r="D73" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="15"/>
-      <c r="F73" s="15" t="s">
+      <c r="F73" t="s">
         <v>34</v>
       </c>
-      <c r="G73" s="15"/>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="2:8">
       <c r="B74" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15" t="s">
+      <c r="D74" t="s">
         <v>40</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" t="s">
         <v>41</v>
       </c>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="2:8">
       <c r="B75" s="4"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="2:8">
       <c r="B76" s="4"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15" t="s">
+      <c r="D76" t="s">
         <v>42</v>
       </c>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15" t="s">
+      <c r="F76" t="s">
         <v>43</v>
       </c>
-      <c r="G76" s="15"/>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="2:8">
       <c r="B77" s="4"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15" t="s">
+      <c r="D77" t="s">
         <v>44</v>
       </c>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15" t="s">
+      <c r="F77" t="s">
         <v>45</v>
       </c>
-      <c r="G77" s="15"/>
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="2:8">
       <c r="B78" s="4"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15" t="s">
+      <c r="D78" t="s">
         <v>60</v>
       </c>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="2:8">
       <c r="B79" s="4"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15" t="s">
+      <c r="D79" t="s">
         <v>46</v>
       </c>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="2:8">
       <c r="B80" s="4"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15" t="s">
+      <c r="D80" t="s">
         <v>47</v>
       </c>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="2:8">
       <c r="B81" s="4"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15" t="s">
+      <c r="D81" t="s">
         <v>48</v>
       </c>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="2:8">
       <c r="B82" s="4"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="15"/>
-      <c r="F82" s="15"/>
-      <c r="G82" s="15"/>
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="2:8">
       <c r="B83" s="4"/>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15" t="s">
+      <c r="D83" t="s">
         <v>49</v>
       </c>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="2:8">
       <c r="B84" s="4"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15" t="s">
+      <c r="D84" t="s">
         <v>46</v>
       </c>
-      <c r="E84" s="15"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="15"/>
       <c r="H84" s="5"/>
     </row>
     <row r="85" spans="2:8">
       <c r="B85" s="4"/>
-      <c r="C85" s="15" t="s">
+      <c r="C85" t="s">
         <v>15</v>
       </c>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="15"/>
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="2:8">
       <c r="B86" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="15"/>
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="2:8">
@@ -11370,394 +11584,114 @@
     </row>
     <row r="132" spans="2:13">
       <c r="B132" s="4"/>
-      <c r="C132" s="15"/>
-      <c r="D132" s="15"/>
-      <c r="E132" s="15"/>
-      <c r="F132" s="15"/>
-      <c r="G132" s="15"/>
-      <c r="H132" s="15"/>
-      <c r="I132" s="15"/>
-      <c r="J132" s="15"/>
-      <c r="K132" s="15"/>
-      <c r="L132" s="15"/>
       <c r="M132" s="5"/>
     </row>
     <row r="133" spans="2:13">
       <c r="B133" s="4"/>
-      <c r="C133" s="15"/>
-      <c r="D133" s="15"/>
-      <c r="E133" s="15"/>
-      <c r="F133" s="15"/>
-      <c r="G133" s="15"/>
-      <c r="H133" s="15"/>
-      <c r="I133" s="15"/>
-      <c r="J133" s="15"/>
-      <c r="K133" s="15"/>
-      <c r="L133" s="15"/>
       <c r="M133" s="5"/>
     </row>
     <row r="134" spans="2:13">
       <c r="B134" s="4"/>
-      <c r="C134" s="15"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
-      <c r="G134" s="15"/>
-      <c r="H134" s="15"/>
-      <c r="I134" s="15"/>
-      <c r="J134" s="15"/>
-      <c r="K134" s="15"/>
-      <c r="L134" s="15"/>
       <c r="M134" s="5"/>
     </row>
     <row r="135" spans="2:13">
       <c r="B135" s="4"/>
-      <c r="C135" s="15"/>
-      <c r="D135" s="15"/>
-      <c r="E135" s="15"/>
-      <c r="F135" s="15"/>
-      <c r="G135" s="15"/>
-      <c r="H135" s="15"/>
-      <c r="I135" s="15"/>
-      <c r="J135" s="15"/>
-      <c r="K135" s="15"/>
-      <c r="L135" s="15"/>
       <c r="M135" s="5"/>
     </row>
     <row r="136" spans="2:13">
       <c r="B136" s="4"/>
-      <c r="C136" s="15"/>
-      <c r="D136" s="15"/>
-      <c r="E136" s="15"/>
-      <c r="F136" s="15"/>
-      <c r="G136" s="15"/>
-      <c r="H136" s="15"/>
-      <c r="I136" s="15"/>
-      <c r="J136" s="15"/>
-      <c r="K136" s="15"/>
-      <c r="L136" s="15"/>
       <c r="M136" s="5"/>
     </row>
     <row r="137" spans="2:13">
       <c r="B137" s="4"/>
-      <c r="C137" s="15"/>
-      <c r="D137" s="15"/>
-      <c r="E137" s="15"/>
-      <c r="F137" s="15"/>
-      <c r="G137" s="15"/>
-      <c r="H137" s="15"/>
-      <c r="I137" s="15"/>
-      <c r="J137" s="15"/>
-      <c r="K137" s="15"/>
-      <c r="L137" s="15"/>
       <c r="M137" s="5"/>
     </row>
     <row r="138" spans="2:13">
       <c r="B138" s="4"/>
-      <c r="C138" s="15"/>
-      <c r="D138" s="15"/>
-      <c r="E138" s="15"/>
-      <c r="F138" s="15"/>
-      <c r="G138" s="15"/>
-      <c r="H138" s="15"/>
-      <c r="I138" s="15"/>
-      <c r="J138" s="15"/>
-      <c r="K138" s="15"/>
-      <c r="L138" s="15"/>
       <c r="M138" s="5"/>
     </row>
     <row r="139" spans="2:13">
       <c r="B139" s="4"/>
-      <c r="C139" s="15"/>
-      <c r="D139" s="15"/>
-      <c r="E139" s="15"/>
-      <c r="F139" s="15"/>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
-      <c r="I139" s="15"/>
-      <c r="J139" s="15"/>
-      <c r="K139" s="15"/>
-      <c r="L139" s="15"/>
       <c r="M139" s="5"/>
     </row>
     <row r="140" spans="2:13">
       <c r="B140" s="4"/>
-      <c r="C140" s="15"/>
-      <c r="D140" s="15"/>
-      <c r="E140" s="15"/>
-      <c r="F140" s="15"/>
-      <c r="G140" s="15"/>
-      <c r="H140" s="15"/>
-      <c r="I140" s="15"/>
-      <c r="J140" s="15"/>
-      <c r="K140" s="15"/>
-      <c r="L140" s="15"/>
       <c r="M140" s="5"/>
     </row>
     <row r="141" spans="2:13">
       <c r="B141" s="4"/>
-      <c r="C141" s="15"/>
-      <c r="D141" s="15"/>
-      <c r="E141" s="15"/>
-      <c r="F141" s="15"/>
-      <c r="G141" s="15"/>
-      <c r="H141" s="15"/>
-      <c r="I141" s="15"/>
-      <c r="J141" s="15"/>
-      <c r="K141" s="15"/>
-      <c r="L141" s="15"/>
       <c r="M141" s="5"/>
     </row>
     <row r="142" spans="2:13">
       <c r="B142" s="4"/>
-      <c r="C142" s="15"/>
-      <c r="D142" s="15"/>
-      <c r="E142" s="15"/>
-      <c r="F142" s="15"/>
-      <c r="G142" s="15"/>
-      <c r="H142" s="15"/>
-      <c r="I142" s="15"/>
-      <c r="J142" s="15"/>
-      <c r="K142" s="15"/>
-      <c r="L142" s="15"/>
       <c r="M142" s="5"/>
     </row>
     <row r="143" spans="2:13">
       <c r="B143" s="4"/>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
-      <c r="G143" s="15"/>
-      <c r="H143" s="15"/>
-      <c r="I143" s="15"/>
-      <c r="J143" s="15"/>
-      <c r="K143" s="15"/>
-      <c r="L143" s="15"/>
       <c r="M143" s="5"/>
     </row>
     <row r="144" spans="2:13">
       <c r="B144" s="4"/>
-      <c r="C144" s="15"/>
-      <c r="D144" s="15"/>
-      <c r="E144" s="15"/>
-      <c r="F144" s="15"/>
-      <c r="G144" s="15"/>
-      <c r="H144" s="15"/>
-      <c r="I144" s="15"/>
-      <c r="J144" s="15"/>
-      <c r="K144" s="15"/>
-      <c r="L144" s="15"/>
       <c r="M144" s="5"/>
     </row>
     <row r="145" spans="2:13">
       <c r="B145" s="4"/>
-      <c r="C145" s="15"/>
-      <c r="D145" s="15"/>
-      <c r="E145" s="15"/>
-      <c r="F145" s="15"/>
-      <c r="G145" s="15"/>
-      <c r="H145" s="15"/>
-      <c r="I145" s="15"/>
-      <c r="J145" s="15"/>
-      <c r="K145" s="15"/>
-      <c r="L145" s="15"/>
       <c r="M145" s="5"/>
     </row>
     <row r="146" spans="2:13">
       <c r="B146" s="4"/>
-      <c r="C146" s="15"/>
-      <c r="D146" s="15"/>
-      <c r="E146" s="15"/>
-      <c r="F146" s="15"/>
-      <c r="G146" s="15"/>
-      <c r="H146" s="15"/>
-      <c r="I146" s="15"/>
-      <c r="J146" s="15"/>
-      <c r="K146" s="15"/>
-      <c r="L146" s="15"/>
       <c r="M146" s="5"/>
     </row>
     <row r="147" spans="2:13">
       <c r="B147" s="4"/>
-      <c r="C147" s="15"/>
-      <c r="D147" s="15"/>
-      <c r="E147" s="15"/>
-      <c r="F147" s="15"/>
-      <c r="G147" s="15"/>
-      <c r="H147" s="15"/>
-      <c r="I147" s="15"/>
-      <c r="J147" s="15"/>
-      <c r="K147" s="15"/>
-      <c r="L147" s="15"/>
       <c r="M147" s="5"/>
     </row>
     <row r="148" spans="2:13">
       <c r="B148" s="4"/>
-      <c r="C148" s="15"/>
-      <c r="D148" s="15"/>
-      <c r="E148" s="15"/>
-      <c r="F148" s="15"/>
-      <c r="G148" s="15"/>
-      <c r="H148" s="15"/>
-      <c r="I148" s="15"/>
-      <c r="J148" s="15"/>
-      <c r="K148" s="15"/>
-      <c r="L148" s="15"/>
       <c r="M148" s="5"/>
     </row>
     <row r="149" spans="2:13">
       <c r="B149" s="4"/>
-      <c r="C149" s="15"/>
-      <c r="D149" s="15"/>
-      <c r="E149" s="15"/>
-      <c r="F149" s="15"/>
-      <c r="G149" s="15"/>
-      <c r="H149" s="15"/>
-      <c r="I149" s="15"/>
-      <c r="J149" s="15"/>
-      <c r="K149" s="15"/>
-      <c r="L149" s="15"/>
       <c r="M149" s="5"/>
     </row>
     <row r="150" spans="2:13">
       <c r="B150" s="4"/>
-      <c r="C150" s="15"/>
-      <c r="D150" s="15"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="15"/>
-      <c r="G150" s="15"/>
-      <c r="H150" s="15"/>
-      <c r="I150" s="15"/>
-      <c r="J150" s="15"/>
-      <c r="K150" s="15"/>
-      <c r="L150" s="15"/>
       <c r="M150" s="5"/>
     </row>
     <row r="151" spans="2:13">
       <c r="B151" s="4"/>
-      <c r="C151" s="15"/>
-      <c r="D151" s="15"/>
-      <c r="E151" s="15"/>
-      <c r="F151" s="15"/>
-      <c r="G151" s="15"/>
-      <c r="H151" s="15"/>
-      <c r="I151" s="15"/>
-      <c r="J151" s="15"/>
-      <c r="K151" s="15"/>
-      <c r="L151" s="15"/>
       <c r="M151" s="5"/>
     </row>
     <row r="152" spans="2:13">
       <c r="B152" s="4"/>
-      <c r="C152" s="15"/>
-      <c r="D152" s="15"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="15"/>
-      <c r="G152" s="15"/>
-      <c r="H152" s="15"/>
-      <c r="I152" s="15"/>
-      <c r="J152" s="15"/>
-      <c r="K152" s="15"/>
-      <c r="L152" s="15"/>
       <c r="M152" s="5"/>
     </row>
     <row r="153" spans="2:13">
       <c r="B153" s="4"/>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-      <c r="G153" s="15"/>
-      <c r="H153" s="15"/>
-      <c r="I153" s="15"/>
-      <c r="J153" s="15"/>
-      <c r="K153" s="15"/>
-      <c r="L153" s="15"/>
       <c r="M153" s="5"/>
     </row>
     <row r="154" spans="2:13">
       <c r="B154" s="4"/>
-      <c r="C154" s="15"/>
-      <c r="D154" s="15"/>
-      <c r="E154" s="15"/>
-      <c r="F154" s="15"/>
-      <c r="G154" s="15"/>
-      <c r="H154" s="15"/>
-      <c r="I154" s="15"/>
-      <c r="J154" s="15"/>
-      <c r="K154" s="15"/>
-      <c r="L154" s="15"/>
       <c r="M154" s="5"/>
     </row>
     <row r="155" spans="2:13">
       <c r="B155" s="4"/>
-      <c r="C155" s="15"/>
-      <c r="D155" s="15"/>
-      <c r="E155" s="15"/>
-      <c r="F155" s="15"/>
-      <c r="G155" s="15"/>
-      <c r="H155" s="15"/>
-      <c r="I155" s="15"/>
-      <c r="J155" s="15"/>
-      <c r="K155" s="15"/>
-      <c r="L155" s="15"/>
       <c r="M155" s="5"/>
     </row>
     <row r="156" spans="2:13">
       <c r="B156" s="4"/>
-      <c r="C156" s="15"/>
-      <c r="D156" s="15"/>
-      <c r="E156" s="15"/>
-      <c r="F156" s="15"/>
-      <c r="G156" s="15"/>
-      <c r="H156" s="15"/>
-      <c r="I156" s="15"/>
-      <c r="J156" s="15"/>
-      <c r="K156" s="15"/>
-      <c r="L156" s="15"/>
       <c r="M156" s="5"/>
     </row>
     <row r="157" spans="2:13">
       <c r="B157" s="4"/>
-      <c r="C157" s="15"/>
-      <c r="D157" s="15"/>
-      <c r="E157" s="15"/>
-      <c r="F157" s="15"/>
-      <c r="G157" s="15"/>
-      <c r="H157" s="15"/>
-      <c r="I157" s="15"/>
-      <c r="J157" s="15"/>
-      <c r="K157" s="15"/>
-      <c r="L157" s="15"/>
       <c r="M157" s="5"/>
     </row>
     <row r="158" spans="2:13">
       <c r="B158" s="4"/>
-      <c r="C158" s="15"/>
-      <c r="D158" s="15"/>
-      <c r="E158" s="15"/>
-      <c r="F158" s="15"/>
-      <c r="G158" s="15"/>
-      <c r="H158" s="15"/>
-      <c r="I158" s="15"/>
-      <c r="J158" s="15"/>
-      <c r="K158" s="15"/>
-      <c r="L158" s="15"/>
       <c r="M158" s="5"/>
     </row>
     <row r="159" spans="2:13">
       <c r="B159" s="4"/>
-      <c r="C159" s="15"/>
-      <c r="D159" s="15"/>
-      <c r="E159" s="15"/>
-      <c r="F159" s="15"/>
-      <c r="G159" s="15"/>
-      <c r="H159" s="15"/>
-      <c r="I159" s="15"/>
-      <c r="J159" s="15"/>
-      <c r="K159" s="15"/>
-      <c r="L159" s="15"/>
       <c r="M159" s="5"/>
     </row>
     <row r="160" spans="2:13">

</xml_diff>